<commit_message>
v1.0.4 (error handling; bug fixes)
</commit_message>
<xml_diff>
--- a/SalesUtil/Copy of SalesUtil_errors.xlsx
+++ b/SalesUtil/Copy of SalesUtil_errors.xlsx
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,47 +587,47 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+    <row r="4" spans="1:3" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="5" spans="1:3" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+    <row r="6" spans="1:3" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+    <row r="7" spans="1:3" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -653,14 +653,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
+    <row r="10" spans="1:3" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -708,8 +708,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:3" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -751,7 +751,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>